<commit_message>
fix tesi + pre v2.1
</commit_message>
<xml_diff>
--- a/altri_doc/Analisi Dati + Modello.xlsx
+++ b/altri_doc/Analisi Dati + Modello.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6180" windowWidth="20535" windowHeight="1170" tabRatio="598" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="6180" windowWidth="20535" windowHeight="1170" tabRatio="598" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Bluetooth" sheetId="9" r:id="rId1"/>
@@ -5373,9 +5373,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.10228765432098766"/>
-          <c:y val="9.896018518518522E-2"/>
-          <c:w val="0.65944027777777792"/>
-          <c:h val="0.79225092592592572"/>
+          <c:y val="9.8960185185185248E-2"/>
+          <c:w val="0.65944027777777814"/>
+          <c:h val="0.79225092592592539"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -5399,80 +5399,193 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.5011377932049746E-2"/>
+                  <c:x val="-3.501137793204976E-2"/>
                   <c:y val="-2.4988820320186029E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>2 KB</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:showCatName val="1"/>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.8626913794513539E-2"/>
+                  <c:x val="-4.8626913794513525E-2"/>
                   <c:y val="-2.7260531258384759E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>800 KB</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:showCatName val="1"/>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-7.7803062071221656E-3"/>
-                  <c:y val="-4.5434218763974596E-3"/>
+                  <c:x val="-7.78030620712217E-3"/>
+                  <c:y val="-4.5434218763974578E-3"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>2MB</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:showCatName val="1"/>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-5.8352296553415527E-3"/>
-                  <c:y val="-2.0445398443788527E-2"/>
+                  <c:x val="-5.8352296553415561E-3"/>
+                  <c:y val="-2.0445398443788544E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>50 MB</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:showCatName val="1"/>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-5.8352296553416247E-3"/>
+                  <c:x val="-5.8352296553416307E-3"/>
                   <c:y val="-2.0445398443788652E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>200 MB</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:showCatName val="1"/>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-7.7803062071221656E-3"/>
+                  <c:x val="-7.78030620712217E-3"/>
                   <c:y val="-2.2717109381987299E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>500 MB</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:showCatName val="1"/>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-9.7253827589027075E-3"/>
+                  <c:x val="-9.7253827589027109E-3"/>
                   <c:y val="-1.5901976567391111E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>800 MB</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showCatName val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>1 GB</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:showCatName val="1"/>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="8"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.3615689018097789E-2"/>
-                  <c:y val="-2.0445398443788568E-2"/>
+                  <c:x val="-1.3615689018097793E-2"/>
+                  <c:y val="-2.0445398443788579E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>5 GB</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:showCatName val="1"/>
             </c:dLbl>
             <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
@@ -6620,11 +6733,11 @@
         <c:dLbls>
           <c:showVal val="1"/>
         </c:dLbls>
-        <c:axId val="84718336"/>
-        <c:axId val="84721024"/>
+        <c:axId val="151409024"/>
+        <c:axId val="151411328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84718336"/>
+        <c:axId val="151409024"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -6653,12 +6766,12 @@
         </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84721024"/>
+        <c:crossAx val="151411328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84721024"/>
+        <c:axId val="151411328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6689,7 +6802,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84718336"/>
+        <c:crossAx val="151409024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6702,7 +6815,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6738,8 +6851,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.10228765432098766"/>
           <c:y val="9.8960185185185248E-2"/>
-          <c:w val="0.65944027777777814"/>
-          <c:h val="0.79225092592592539"/>
+          <c:w val="0.65944027777777836"/>
+          <c:h val="0.79225092592592516"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -6760,13 +6873,66 @@
           </c:tx>
           <c:dLbls>
             <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>2 KB</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showCatName val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>800 KB</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showCatName val="1"/>
+            </c:dLbl>
+            <c:dLbl>
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.2317901234567901E-2"/>
-                  <c:y val="-9.6485185185184973E-3"/>
+                  <c:x val="-1.2317901234567904E-2"/>
+                  <c:y val="-9.6485185185185007E-3"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>2</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> MB</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:dLblPos val="r"/>
               <c:showCatName val="1"/>
             </c:dLbl>
@@ -6774,10 +6940,22 @@
               <c:idx val="3"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.4277932098765432E-2"/>
-                  <c:y val="-2.1407777777777734E-2"/>
+                  <c:x val="-1.4277932098765433E-2"/>
+                  <c:y val="-2.1407777777777762E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>50 MB</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:dLblPos val="r"/>
               <c:showCatName val="1"/>
             </c:dLbl>
@@ -6785,10 +6963,22 @@
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-5.5879629629629628E-4"/>
-                  <c:y val="-1.200037037037037E-2"/>
+                  <c:x val="-5.5879629629629649E-4"/>
+                  <c:y val="-1.2000370370370371E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>200 MB</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:dLblPos val="r"/>
               <c:showCatName val="1"/>
             </c:dLbl>
@@ -6797,9 +6987,21 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-1.4277777777777849E-2"/>
-                  <c:y val="-3.0815185185185185E-2"/>
+                  <c:y val="-3.0815185185185195E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>500 MB</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:dLblPos val="r"/>
               <c:showCatName val="1"/>
             </c:dLbl>
@@ -6807,10 +7009,22 @@
               <c:idx val="6"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.2317901234567901E-2"/>
-                  <c:y val="-2.3759629629629631E-2"/>
+                  <c:x val="-1.2317901234567904E-2"/>
+                  <c:y val="-2.3759629629629637E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>800 MB</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:dLblPos val="r"/>
               <c:showCatName val="1"/>
             </c:dLbl>
@@ -6818,10 +7032,22 @@
               <c:idx val="7"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-5.5864197530864203E-4"/>
-                  <c:y val="2.1107407407407407E-3"/>
+                  <c:x val="-5.5864197530864225E-4"/>
+                  <c:y val="2.110740740740742E-3"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>1 GB</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:dLblPos val="r"/>
               <c:showCatName val="1"/>
             </c:dLbl>
@@ -6829,10 +7055,22 @@
               <c:idx val="8"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.6237654320987654E-2"/>
-                  <c:y val="-1.4352222222222223E-2"/>
+                  <c:x val="-1.6237654320987661E-2"/>
+                  <c:y val="-1.4352222222222219E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>5 GB</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:dLblPos val="r"/>
               <c:showCatName val="1"/>
             </c:dLbl>
@@ -7912,11 +8150,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="85840256"/>
-        <c:axId val="85842176"/>
+        <c:axId val="151572480"/>
+        <c:axId val="151574400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85840256"/>
+        <c:axId val="151572480"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7945,12 +8183,12 @@
         </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85842176"/>
+        <c:crossAx val="151574400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85842176"/>
+        <c:axId val="151574400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7976,7 +8214,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85840256"/>
+        <c:crossAx val="151572480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7989,7 +8227,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8031,13 +8269,94 @@
           <c:order val="0"/>
           <c:dLbls>
             <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.739387480311387E-2"/>
+                  <c:y val="-1.9087271467291101E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>10 B</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showCatName val="1"/>
+            </c:dLbl>
+            <c:dLbl>
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.5836425283398962E-2"/>
-                  <c:y val="2.7955009415282988E-2"/>
+                  <c:x val="-3.1954884632788165E-2"/>
+                  <c:y val="-1.9159426999747077E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>30 B</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showCatName val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.2313831335729609E-2"/>
+                  <c:y val="-1.6731550998936771E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>300 B</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showCatName val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.1396774055026802E-2"/>
+                  <c:y val="-1.6731550998936771E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>2 KB</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:dLblPos val="r"/>
               <c:showCatName val="1"/>
             </c:dLbl>
@@ -8045,10 +8364,22 @@
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-8.1050784112775331E-2"/>
-                  <c:y val="-2.1387807902325272E-2"/>
+                  <c:x val="-7.7169277526656324E-2"/>
+                  <c:y val="-1.1964834101632087E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>800 KB</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:dLblPos val="r"/>
               <c:showCatName val="1"/>
             </c:dLbl>
@@ -8056,10 +8387,22 @@
               <c:idx val="5"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-6.5754639776950579E-3"/>
-                  <c:y val="2.1087717727262803E-3"/>
+                  <c:x val="-5.8976517618242852E-2"/>
+                  <c:y val="-1.4381209734801522E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>2 MB</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:dLblPos val="r"/>
               <c:showCatName val="1"/>
             </c:dLbl>
@@ -8067,10 +8410,22 @@
               <c:idx val="6"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-8.8753100116219147E-2"/>
-                  <c:y val="-1.6688491967315006E-2"/>
+                  <c:x val="-8.8753100116219216E-2"/>
+                  <c:y val="-1.6688491967315013E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>50 MB</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:dLblPos val="r"/>
               <c:showCatName val="1"/>
             </c:dLbl>
@@ -8078,10 +8433,22 @@
               <c:idx val="7"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.9956794746418942E-2"/>
-                  <c:y val="3.7353641285303614E-2"/>
+                  <c:x val="-8.8180230408922575E-2"/>
+                  <c:y val="-3.3796241679854991E-4"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>200 MB</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:dLblPos val="r"/>
               <c:showCatName val="1"/>
             </c:dLbl>
@@ -8089,10 +8456,22 @@
               <c:idx val="8"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-8.6793223270559147E-2"/>
-                  <c:y val="-2.1387807902325272E-2"/>
+                  <c:x val="-9.0674821818719734E-2"/>
+                  <c:y val="-1.8623175986045231E-4"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>500 MB</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:dLblPos val="r"/>
               <c:showCatName val="1"/>
             </c:dLbl>
@@ -8100,10 +8479,22 @@
               <c:idx val="9"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.4783957528388508E-3"/>
-                  <c:y val="2.5605351447777834E-2"/>
+                  <c:x val="-8.2816186481252288E-2"/>
+                  <c:y val="-7.2533931649234338E-3"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>800 MB</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:dLblPos val="r"/>
               <c:showCatName val="1"/>
             </c:dLbl>
@@ -8111,10 +8502,22 @@
               <c:idx val="10"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-5.7395070585659042E-2"/>
-                  <c:y val="-3.3136097739851052E-2"/>
+                  <c:x val="-5.3475243655899812E-2"/>
+                  <c:y val="-1.9019938669652309E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>1 GB</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:dLblPos val="r"/>
               <c:showCatName val="1"/>
             </c:dLbl>
@@ -8122,10 +8525,27 @@
               <c:idx val="11"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-6.1476244054975933E-2"/>
-                  <c:y val="-2.843678180484074E-2"/>
+                  <c:x val="-5.7193596889371041E-2"/>
+                  <c:y val="-1.4326675733408123E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>5</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> GB</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:dLblPos val="r"/>
               <c:showCatName val="1"/>
             </c:dLbl>
@@ -8227,11 +8647,11 @@
         <c:dLbls>
           <c:showVal val="1"/>
         </c:dLbls>
-        <c:axId val="88756608"/>
-        <c:axId val="88758528"/>
+        <c:axId val="153624960"/>
+        <c:axId val="153626880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88756608"/>
+        <c:axId val="153624960"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -8264,12 +8684,12 @@
         <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88758528"/>
-        <c:crossesAt val="1.0000000000000007E-3"/>
+        <c:crossAx val="153626880"/>
+        <c:crossesAt val="1.0000000000000011E-3"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88758528"/>
+        <c:axId val="153626880"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -8297,7 +8717,7 @@
         <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88756608"/>
+        <c:crossAx val="153624960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8306,7 +8726,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8432,11 +8852,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="91621632"/>
-        <c:axId val="91636096"/>
+        <c:axId val="153647744"/>
+        <c:axId val="153678208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91621632"/>
+        <c:axId val="153647744"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -8469,12 +8889,12 @@
         <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91636096"/>
-        <c:crossesAt val="1.0000000000000011E-3"/>
+        <c:crossAx val="153678208"/>
+        <c:crossesAt val="1.0000000000000015E-3"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91636096"/>
+        <c:axId val="153678208"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -8510,7 +8930,7 @@
         <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91621632"/>
+        <c:crossAx val="153647744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8519,7 +8939,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8537,7 +8957,7 @@
     <xdr:to>
       <xdr:col>38</xdr:col>
       <xdr:colOff>372794</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>99617</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8700,9 +9120,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>59</xdr:col>
-      <xdr:colOff>357104</xdr:colOff>
+      <xdr:colOff>277864</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>37425</xdr:rowOff>
+      <xdr:rowOff>25178</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9093,7 +9513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:U47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="X32" sqref="X32"/>
     </sheetView>
   </sheetViews>
@@ -9996,8 +10416,8 @@
   <sheetPr codeName="Foglio1"/>
   <dimension ref="A1:AU31"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AN31" sqref="AN31"/>
+    <sheetView topLeftCell="R1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AW4" sqref="AW4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12657,8 +13077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BA9" sqref="BA9"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AY25" sqref="AY25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16351,7 +16771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AZ43"/>
   <sheetViews>
-    <sheetView topLeftCell="AV3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AV1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AV28" sqref="AV28"/>
     </sheetView>
   </sheetViews>

</xml_diff>